<commit_message>
update pdf - 1
</commit_message>
<xml_diff>
--- a/src/NhapNoiThat.xlsx
+++ b/src/NhapNoiThat.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NAMFORK\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a3a683147dce32a0/Desktop/Data/code/Java/BuildingOperationsApplication/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21088153-C936-49DB-8EAC-086FEE060D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{21088153-C936-49DB-8EAC-086FEE060D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4B37307-5BAB-40B3-8596-34DA480BA9E6}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="9615" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3795" yWindow="0" windowWidth="14400" windowHeight="8722" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -111,7 +111,7 @@
     <t>mới</t>
   </si>
   <si>
-    <t>nameFurniture</t>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -122,7 +122,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -134,7 +134,7 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -447,16 +447,16 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.125" customWidth="1"/>
+    <col min="2" max="2" width="14.125" customWidth="1"/>
+    <col min="3" max="3" width="23.4375" customWidth="1"/>
+    <col min="4" max="4" width="17.3125" customWidth="1"/>
+    <col min="5" max="5" width="10.6875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>